<commit_message>
Driver updated to catch SerialPort Exception and new Metadata tags added.
</commit_message>
<xml_diff>
--- a/RaspberryPiList.xlsx
+++ b/RaspberryPiList.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="62">
   <si>
     <t>RasPi Name</t>
   </si>
@@ -121,6 +121,18 @@
     <t>b8:27:eb:7d:8a:2e</t>
   </si>
   <si>
+    <t>AB-RPi02</t>
+  </si>
+  <si>
+    <t>192.168.136.58</t>
+  </si>
+  <si>
+    <t>b8:27:eb:8b:bc:a4</t>
+  </si>
+  <si>
+    <t>Deployed, not configured</t>
+  </si>
+  <si>
     <t>LB-RPi01</t>
   </si>
   <si>
@@ -191,9 +203,6 @@
   </si>
   <si>
     <t>b8:27:eb:01:74:0a</t>
-  </si>
-  <si>
-    <t>To be Deployed</t>
   </si>
 </sst>
 </file>
@@ -206,6 +215,7 @@
   <fonts count="4">
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -286,22 +296,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D14" activeCellId="0" pane="topLeft" sqref="D14"/>
+      <selection activeCell="E10" activeCellId="0" pane="topLeft" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.0823529411765"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.0196078431373"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.8313725490196"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.4980392156863"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.878431372549"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1921568627451"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.1725490196078"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.956862745098"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.6078431372549"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.9960784313725"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -318,7 +328,7 @@
         <v>4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
         <v>5</v>
       </c>
@@ -335,7 +345,7 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
         <v>10</v>
       </c>
@@ -352,7 +362,7 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
         <v>14</v>
       </c>
@@ -369,7 +379,7 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
         <v>18</v>
       </c>
@@ -386,7 +396,7 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
         <v>22</v>
       </c>
@@ -403,7 +413,7 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
         <v>26</v>
       </c>
@@ -420,7 +430,7 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="8">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="8">
       <c r="A8" s="0" t="s">
         <v>30</v>
       </c>
@@ -437,24 +447,24 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="9">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
         <v>34</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="D9" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="E9" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="10">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="10">
       <c r="A10" s="0" t="s">
         <v>38</v>
       </c>
@@ -471,7 +481,7 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="11">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="11">
       <c r="A11" s="0" t="s">
         <v>42</v>
       </c>
@@ -488,7 +498,7 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="12">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="12">
       <c r="A12" s="0" t="s">
         <v>46</v>
       </c>
@@ -505,7 +515,7 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="13">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="13">
       <c r="A13" s="0" t="s">
         <v>50</v>
       </c>
@@ -522,7 +532,7 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="14">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="14">
       <c r="A14" s="0" t="s">
         <v>54</v>
       </c>
@@ -536,7 +546,24 @@
         <v>57</v>
       </c>
       <c r="E14" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="15">
+      <c r="A15" s="0" t="s">
         <v>58</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -557,17 +584,17 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -582,17 +609,17 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Modified RateActuation utility to accomodate duplicate Meter IDs. Fixed to work with Faculty Housing. IP-List and RaspberryPiList updated with new deployments.
</commit_message>
<xml_diff>
--- a/RaspberryPiList.xlsx
+++ b/RaspberryPiList.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="198" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="152" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="68">
   <si>
     <t>RasPi Name</t>
   </si>
@@ -130,9 +130,6 @@
     <t>b8:27:eb:8b:bc:a4</t>
   </si>
   <si>
-    <t>Deployed, not configured</t>
-  </si>
-  <si>
     <t>LB-RPi01</t>
   </si>
   <si>
@@ -203,6 +200,27 @@
   </si>
   <si>
     <t>b8:27:eb:01:74:0a</t>
+  </si>
+  <si>
+    <t>FB-RPi01</t>
+  </si>
+  <si>
+    <t>Service Block – Lower Ground Floor</t>
+  </si>
+  <si>
+    <t>192.168.136.57</t>
+  </si>
+  <si>
+    <t>b8:27:eb:73:d1:fd</t>
+  </si>
+  <si>
+    <t>Service Block – Upper Ground Floor</t>
+  </si>
+  <si>
+    <t>192.168.136.59</t>
+  </si>
+  <si>
+    <t>b8:27:eb:8d:2a:44</t>
   </si>
 </sst>
 </file>
@@ -296,19 +314,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E10" activeCellId="0" pane="topLeft" sqref="E10"/>
+      <selection activeCell="D17" activeCellId="0" pane="topLeft" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1921568627451"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.1725490196078"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.956862745098"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.6078431372549"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.9960784313725"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.2980392156863"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.3254901960784"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.0941176470588"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.7137254901961"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.1137254901961"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.6941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="1">
@@ -461,21 +479,21 @@
         <v>36</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="10">
       <c r="A10" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="C10" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="D10" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>41</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>9</v>
@@ -483,16 +501,16 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="11">
       <c r="A11" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="C11" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="D11" s="0" t="s">
         <v>44</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>45</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>9</v>
@@ -500,16 +518,16 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="12">
       <c r="A12" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="C12" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="D12" s="0" t="s">
         <v>48</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>49</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>9</v>
@@ -517,16 +535,16 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="13">
       <c r="A13" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="C13" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="D13" s="0" t="s">
         <v>52</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>53</v>
       </c>
       <c r="E13" s="0" t="s">
         <v>9</v>
@@ -534,35 +552,69 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="14">
       <c r="A14" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="C14" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="D14" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="E14" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.55" outlineLevel="0" r="15">
+      <c r="A15" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="E14" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="15">
-      <c r="A15" s="0" t="s">
+      <c r="B15" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="C15" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="D15" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="E15" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="16">
+      <c r="A16" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="B16" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="17">
+      <c r="A17" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="0" t="s">
         <v>9</v>
       </c>
     </row>
@@ -589,7 +641,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6941176470588"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -614,7 +666,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6941176470588"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>